<commit_message>
Prod Move issues fixed
</commit_message>
<xml_diff>
--- a/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormWD.xlsx
+++ b/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormWD.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VARADHA\source\repos\jayanthkundety\RAMMS2.0\RAMS\Web\RAMMS.Web.UI\wwwroot\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Form WD" sheetId="4" r:id="rId1"/>
@@ -247,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -277,21 +277,48 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -301,35 +328,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -368,7 +371,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2CAA98BF-11A6-4330-B3ED-ACEC4BC59997}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CAA98BF-11A6-4330-B3ED-ACEC4BC59997}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -799,53 +802,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AO54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="T40" sqref="T40:Y40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:AF12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="0.7265625" style="1" customWidth="1"/>
-    <col min="2" max="32" width="2.7265625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="0.54296875" style="1" customWidth="1"/>
-    <col min="34" max="42" width="2.7265625" style="1" customWidth="1"/>
-    <col min="43" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="0.7109375" style="1" customWidth="1"/>
+    <col min="2" max="18" width="2.7109375" style="1" customWidth="1"/>
+    <col min="19" max="20" width="3.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="5.140625" style="1" customWidth="1"/>
+    <col min="22" max="32" width="2.7109375" style="1" customWidth="1"/>
+    <col min="33" max="33" width="0.5703125" style="1" customWidth="1"/>
+    <col min="34" max="42" width="2.7109375" style="1" customWidth="1"/>
+    <col min="43" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:41" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="AB2" s="16" t="s">
+    <row r="1" spans="2:41" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:41" ht="15" x14ac:dyDescent="0.25">
+      <c r="AB2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="16"/>
-      <c r="AF2" s="16"/>
-    </row>
-    <row r="4" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+    </row>
+    <row r="4" spans="2:41" ht="15" x14ac:dyDescent="0.25">
       <c r="K4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:41" x14ac:dyDescent="0.2">
       <c r="K5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:41" x14ac:dyDescent="0.2">
       <c r="K6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:41" x14ac:dyDescent="0.2">
       <c r="K7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="2:41" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -878,143 +884,143 @@
       <c r="AE8" s="6"/>
       <c r="AF8" s="6"/>
     </row>
-    <row r="9" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="17"/>
-      <c r="W9" s="17"/>
-      <c r="X9" s="17"/>
-      <c r="Y9" s="17"/>
-      <c r="Z9" s="17"/>
-      <c r="AA9" s="17"/>
-      <c r="AB9" s="17"/>
-      <c r="AC9" s="17"/>
-      <c r="AD9" s="17"/>
-      <c r="AE9" s="17"/>
-      <c r="AF9" s="17"/>
-    </row>
-    <row r="10" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B10" s="18" t="s">
+    <row r="9" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="32"/>
+      <c r="AA9" s="32"/>
+      <c r="AB9" s="32"/>
+      <c r="AC9" s="32"/>
+      <c r="AD9" s="32"/>
+      <c r="AE9" s="32"/>
+      <c r="AF9" s="32"/>
+    </row>
+    <row r="10" spans="2:41" x14ac:dyDescent="0.2">
+      <c r="B10" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="18"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="18"/>
-      <c r="AC10" s="18"/>
-      <c r="AD10" s="18"/>
-      <c r="AE10" s="18"/>
-      <c r="AF10" s="18"/>
-      <c r="AG10" s="18"/>
-    </row>
-    <row r="11" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-      <c r="AC11" s="18"/>
-      <c r="AD11" s="18"/>
-      <c r="AE11" s="18"/>
-      <c r="AF11" s="18"/>
-      <c r="AG11" s="18"/>
-    </row>
-    <row r="12" spans="2:41" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="19"/>
-      <c r="W12" s="19"/>
-      <c r="X12" s="19"/>
-      <c r="Y12" s="19"/>
-      <c r="Z12" s="19"/>
-      <c r="AA12" s="19"/>
-      <c r="AB12" s="19"/>
-      <c r="AC12" s="19"/>
-      <c r="AD12" s="19"/>
-      <c r="AE12" s="19"/>
-      <c r="AF12" s="19"/>
-    </row>
-    <row r="14" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="28"/>
+      <c r="AB10" s="28"/>
+      <c r="AC10" s="28"/>
+      <c r="AD10" s="28"/>
+      <c r="AE10" s="28"/>
+      <c r="AF10" s="28"/>
+      <c r="AG10" s="28"/>
+    </row>
+    <row r="11" spans="2:41" x14ac:dyDescent="0.2">
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="28"/>
+      <c r="X11" s="28"/>
+      <c r="Y11" s="28"/>
+      <c r="Z11" s="28"/>
+      <c r="AA11" s="28"/>
+      <c r="AB11" s="28"/>
+      <c r="AC11" s="28"/>
+      <c r="AD11" s="28"/>
+      <c r="AE11" s="28"/>
+      <c r="AF11" s="28"/>
+      <c r="AG11" s="28"/>
+    </row>
+    <row r="12" spans="2:41" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="33"/>
+      <c r="U12" s="33"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="33"/>
+      <c r="X12" s="33"/>
+      <c r="Y12" s="33"/>
+      <c r="Z12" s="33"/>
+      <c r="AA12" s="33"/>
+      <c r="AB12" s="33"/>
+      <c r="AC12" s="33"/>
+      <c r="AD12" s="33"/>
+      <c r="AE12" s="33"/>
+      <c r="AF12" s="33"/>
+    </row>
+    <row r="14" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
@@ -1023,13 +1029,13 @@
       <c r="E14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1044,23 +1050,23 @@
       </c>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
-      <c r="Y14" s="21"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="15"/>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="15"/>
-      <c r="AF14" s="15"/>
-      <c r="AI14" s="22"/>
-      <c r="AJ14" s="22"/>
-      <c r="AK14" s="22"/>
-      <c r="AL14" s="22"/>
-      <c r="AM14" s="22"/>
-      <c r="AN14" s="22"/>
-      <c r="AO14" s="22"/>
-    </row>
-    <row r="15" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="21"/>
+      <c r="AA14" s="21"/>
+      <c r="AB14" s="21"/>
+      <c r="AC14" s="21"/>
+      <c r="AD14" s="21"/>
+      <c r="AE14" s="21"/>
+      <c r="AF14" s="21"/>
+      <c r="AI14" s="31"/>
+      <c r="AJ14" s="31"/>
+      <c r="AK14" s="31"/>
+      <c r="AL14" s="31"/>
+      <c r="AM14" s="31"/>
+      <c r="AN14" s="31"/>
+      <c r="AO14" s="31"/>
+    </row>
+    <row r="15" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -1069,13 +1075,13 @@
       <c r="E15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -1096,26 +1102,26 @@
       <c r="AD15" s="4"/>
       <c r="AE15" s="4"/>
       <c r="AF15" s="4"/>
-      <c r="AH15" s="15"/>
-      <c r="AI15" s="15"/>
-      <c r="AJ15" s="15"/>
-      <c r="AK15" s="15"/>
-      <c r="AL15" s="15"/>
-      <c r="AM15" s="15"/>
-      <c r="AN15" s="15"/>
-    </row>
-    <row r="16" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="AH15" s="21"/>
+      <c r="AI15" s="21"/>
+      <c r="AJ15" s="21"/>
+      <c r="AK15" s="21"/>
+      <c r="AL15" s="21"/>
+      <c r="AM15" s="21"/>
+      <c r="AN15" s="21"/>
+    </row>
+    <row r="16" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -1137,7 +1143,7 @@
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
     </row>
-    <row r="17" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1170,7 +1176,7 @@
       <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
     </row>
-    <row r="18" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1202,15 +1208,15 @@
       <c r="AD18" s="4"/>
       <c r="AE18" s="4"/>
       <c r="AF18" s="4"/>
-      <c r="AH18" s="15"/>
-      <c r="AI18" s="15"/>
-      <c r="AJ18" s="15"/>
-      <c r="AK18" s="15"/>
-      <c r="AL18" s="15"/>
-      <c r="AM18" s="15"/>
-      <c r="AN18" s="15"/>
-    </row>
-    <row r="19" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="AH18" s="21"/>
+      <c r="AI18" s="21"/>
+      <c r="AJ18" s="21"/>
+      <c r="AK18" s="21"/>
+      <c r="AL18" s="21"/>
+      <c r="AM18" s="21"/>
+      <c r="AN18" s="21"/>
+    </row>
+    <row r="19" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1242,15 +1248,15 @@
       <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
       <c r="AF19" s="4"/>
-      <c r="AH19" s="15"/>
-      <c r="AI19" s="15"/>
-      <c r="AJ19" s="15"/>
-      <c r="AK19" s="15"/>
-      <c r="AL19" s="15"/>
-      <c r="AM19" s="15"/>
-      <c r="AN19" s="15"/>
-    </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="AH19" s="21"/>
+      <c r="AI19" s="21"/>
+      <c r="AJ19" s="21"/>
+      <c r="AK19" s="21"/>
+      <c r="AL19" s="21"/>
+      <c r="AM19" s="21"/>
+      <c r="AN19" s="21"/>
+    </row>
+    <row r="20" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1282,15 +1288,15 @@
       <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
-      <c r="AH20" s="15"/>
-      <c r="AI20" s="15"/>
-      <c r="AJ20" s="15"/>
-      <c r="AK20" s="15"/>
-      <c r="AL20" s="15"/>
-      <c r="AM20" s="15"/>
-      <c r="AN20" s="15"/>
-    </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="AH20" s="21"/>
+      <c r="AI20" s="21"/>
+      <c r="AJ20" s="21"/>
+      <c r="AK20" s="21"/>
+      <c r="AL20" s="21"/>
+      <c r="AM20" s="21"/>
+      <c r="AN20" s="21"/>
+    </row>
+    <row r="21" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1322,15 +1328,15 @@
       <c r="AD21" s="4"/>
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
-      <c r="AH21" s="15"/>
-      <c r="AI21" s="15"/>
-      <c r="AJ21" s="15"/>
-      <c r="AK21" s="15"/>
-      <c r="AL21" s="15"/>
-      <c r="AM21" s="15"/>
-      <c r="AN21" s="15"/>
-    </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="AH21" s="21"/>
+      <c r="AI21" s="21"/>
+      <c r="AJ21" s="21"/>
+      <c r="AK21" s="21"/>
+      <c r="AL21" s="21"/>
+      <c r="AM21" s="21"/>
+      <c r="AN21" s="21"/>
+    </row>
+    <row r="22" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1363,7 +1369,7 @@
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
     </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1395,15 +1401,15 @@
       <c r="AD23" s="4"/>
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
-      <c r="AH23" s="15"/>
-      <c r="AI23" s="15"/>
-      <c r="AJ23" s="15"/>
-      <c r="AK23" s="15"/>
-      <c r="AL23" s="15"/>
-      <c r="AM23" s="15"/>
-      <c r="AN23" s="15"/>
-    </row>
-    <row r="24" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="AH23" s="21"/>
+      <c r="AI23" s="21"/>
+      <c r="AJ23" s="21"/>
+      <c r="AK23" s="21"/>
+      <c r="AL23" s="21"/>
+      <c r="AM23" s="21"/>
+      <c r="AN23" s="21"/>
+    </row>
+    <row r="24" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1435,15 +1441,15 @@
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
       <c r="AF24" s="4"/>
-      <c r="AH24" s="15"/>
-      <c r="AI24" s="15"/>
-      <c r="AJ24" s="15"/>
-      <c r="AK24" s="15"/>
-      <c r="AL24" s="15"/>
-      <c r="AM24" s="15"/>
-      <c r="AN24" s="15"/>
-    </row>
-    <row r="25" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="AH24" s="21"/>
+      <c r="AI24" s="21"/>
+      <c r="AJ24" s="21"/>
+      <c r="AK24" s="21"/>
+      <c r="AL24" s="21"/>
+      <c r="AM24" s="21"/>
+      <c r="AN24" s="21"/>
+    </row>
+    <row r="25" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1476,98 +1482,98 @@
       <c r="AE25" s="4"/>
       <c r="AF25" s="4"/>
     </row>
-    <row r="26" spans="2:40" s="8" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:40" s="8" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
-      <c r="X26" s="23"/>
-      <c r="Y26" s="23"/>
-      <c r="Z26" s="23"/>
-      <c r="AA26" s="23"/>
-      <c r="AB26" s="23"/>
-      <c r="AC26" s="23"/>
-      <c r="AD26" s="23"/>
-      <c r="AE26" s="23"/>
-      <c r="AF26" s="23"/>
-      <c r="AH26" s="15"/>
-      <c r="AI26" s="15"/>
-      <c r="AJ26" s="15"/>
-      <c r="AK26" s="15"/>
-      <c r="AL26" s="15"/>
-      <c r="AM26" s="15"/>
-      <c r="AN26" s="15"/>
-    </row>
-    <row r="27" spans="2:40" s="8" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="26"/>
+      <c r="AA26" s="26"/>
+      <c r="AB26" s="26"/>
+      <c r="AC26" s="26"/>
+      <c r="AD26" s="26"/>
+      <c r="AE26" s="26"/>
+      <c r="AF26" s="26"/>
+      <c r="AH26" s="21"/>
+      <c r="AI26" s="21"/>
+      <c r="AJ26" s="21"/>
+      <c r="AK26" s="21"/>
+      <c r="AL26" s="21"/>
+      <c r="AM26" s="21"/>
+      <c r="AN26" s="21"/>
+    </row>
+    <row r="27" spans="2:40" s="8" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
-      <c r="T27" s="24"/>
-      <c r="U27" s="24"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="24"/>
-      <c r="X27" s="24"/>
-      <c r="Y27" s="24"/>
-      <c r="Z27" s="24"/>
-      <c r="AA27" s="24"/>
-      <c r="AB27" s="24"/>
-      <c r="AC27" s="24"/>
-      <c r="AD27" s="24"/>
-      <c r="AE27" s="24"/>
-      <c r="AF27" s="24"/>
-    </row>
-    <row r="28" spans="2:40" s="8" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="24"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="24"/>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="24"/>
-      <c r="Z28" s="24"/>
-      <c r="AA28" s="24"/>
-      <c r="AB28" s="24"/>
-      <c r="AC28" s="24"/>
-      <c r="AD28" s="24"/>
-      <c r="AE28" s="24"/>
-      <c r="AF28" s="24"/>
-    </row>
-    <row r="29" spans="2:40" s="8" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="23"/>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="23"/>
+      <c r="Z27" s="23"/>
+      <c r="AA27" s="23"/>
+      <c r="AB27" s="23"/>
+      <c r="AC27" s="23"/>
+      <c r="AD27" s="23"/>
+      <c r="AE27" s="23"/>
+      <c r="AF27" s="23"/>
+    </row>
+    <row r="28" spans="2:40" s="8" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="23"/>
+      <c r="X28" s="23"/>
+      <c r="Y28" s="23"/>
+      <c r="Z28" s="23"/>
+      <c r="AA28" s="23"/>
+      <c r="AB28" s="23"/>
+      <c r="AC28" s="23"/>
+      <c r="AD28" s="23"/>
+      <c r="AE28" s="23"/>
+      <c r="AF28" s="23"/>
+    </row>
+    <row r="29" spans="2:40" s="8" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -1593,178 +1599,178 @@
       <c r="AE29" s="9"/>
       <c r="AF29" s="9"/>
     </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-      <c r="P30" s="25"/>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="25"/>
-      <c r="T30" s="25"/>
-      <c r="U30" s="25"/>
-      <c r="V30" s="25"/>
-      <c r="W30" s="25"/>
-      <c r="X30" s="25"/>
-      <c r="Y30" s="25"/>
-      <c r="Z30" s="25"/>
-      <c r="AA30" s="25"/>
-      <c r="AB30" s="25"/>
-      <c r="AC30" s="25"/>
-      <c r="AD30" s="25"/>
-      <c r="AE30" s="25"/>
-      <c r="AF30" s="25"/>
-    </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="25"/>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="25"/>
-      <c r="T31" s="25"/>
-      <c r="U31" s="25"/>
-      <c r="V31" s="25"/>
-      <c r="W31" s="25"/>
-      <c r="X31" s="25"/>
-      <c r="Y31" s="25"/>
-      <c r="Z31" s="25"/>
-      <c r="AA31" s="25"/>
-      <c r="AB31" s="25"/>
-      <c r="AC31" s="25"/>
-      <c r="AD31" s="25"/>
-      <c r="AE31" s="25"/>
-      <c r="AF31" s="25"/>
-    </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="25"/>
-      <c r="P32" s="25"/>
-      <c r="Q32" s="25"/>
-      <c r="R32" s="25"/>
-      <c r="S32" s="25"/>
-      <c r="T32" s="25"/>
-      <c r="U32" s="25"/>
-      <c r="V32" s="25"/>
-      <c r="W32" s="25"/>
-      <c r="X32" s="25"/>
-      <c r="Y32" s="25"/>
-      <c r="Z32" s="25"/>
-      <c r="AA32" s="25"/>
-      <c r="AB32" s="25"/>
-      <c r="AC32" s="25"/>
-      <c r="AD32" s="25"/>
-      <c r="AE32" s="25"/>
-      <c r="AF32" s="25"/>
-    </row>
-    <row r="33" spans="2:32" ht="5.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="25"/>
-      <c r="P33" s="25"/>
-      <c r="Q33" s="25"/>
-      <c r="R33" s="25"/>
-      <c r="S33" s="25"/>
-      <c r="T33" s="25"/>
-      <c r="U33" s="25"/>
-      <c r="V33" s="25"/>
-      <c r="W33" s="25"/>
-      <c r="X33" s="25"/>
-      <c r="Y33" s="25"/>
-      <c r="Z33" s="25"/>
-      <c r="AA33" s="25"/>
-      <c r="AB33" s="25"/>
-      <c r="AC33" s="25"/>
-      <c r="AD33" s="25"/>
-      <c r="AE33" s="25"/>
-      <c r="AF33" s="25"/>
-    </row>
-    <row r="34" spans="2:32" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="26" t="s">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="24"/>
+      <c r="R30" s="24"/>
+      <c r="S30" s="24"/>
+      <c r="T30" s="24"/>
+      <c r="U30" s="24"/>
+      <c r="V30" s="24"/>
+      <c r="W30" s="24"/>
+      <c r="X30" s="24"/>
+      <c r="Y30" s="24"/>
+      <c r="Z30" s="24"/>
+      <c r="AA30" s="24"/>
+      <c r="AB30" s="24"/>
+      <c r="AC30" s="24"/>
+      <c r="AD30" s="24"/>
+      <c r="AE30" s="24"/>
+      <c r="AF30" s="24"/>
+    </row>
+    <row r="31" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24"/>
+      <c r="S31" s="24"/>
+      <c r="T31" s="24"/>
+      <c r="U31" s="24"/>
+      <c r="V31" s="24"/>
+      <c r="W31" s="24"/>
+      <c r="X31" s="24"/>
+      <c r="Y31" s="24"/>
+      <c r="Z31" s="24"/>
+      <c r="AA31" s="24"/>
+      <c r="AB31" s="24"/>
+      <c r="AC31" s="24"/>
+      <c r="AD31" s="24"/>
+      <c r="AE31" s="24"/>
+      <c r="AF31" s="24"/>
+    </row>
+    <row r="32" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
+      <c r="S32" s="24"/>
+      <c r="T32" s="24"/>
+      <c r="U32" s="24"/>
+      <c r="V32" s="24"/>
+      <c r="W32" s="24"/>
+      <c r="X32" s="24"/>
+      <c r="Y32" s="24"/>
+      <c r="Z32" s="24"/>
+      <c r="AA32" s="24"/>
+      <c r="AB32" s="24"/>
+      <c r="AC32" s="24"/>
+      <c r="AD32" s="24"/>
+      <c r="AE32" s="24"/>
+      <c r="AF32" s="24"/>
+    </row>
+    <row r="33" spans="2:32" ht="5.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="24"/>
+      <c r="T33" s="24"/>
+      <c r="U33" s="24"/>
+      <c r="V33" s="24"/>
+      <c r="W33" s="24"/>
+      <c r="X33" s="24"/>
+      <c r="Y33" s="24"/>
+      <c r="Z33" s="24"/>
+      <c r="AA33" s="24"/>
+      <c r="AB33" s="24"/>
+      <c r="AC33" s="24"/>
+      <c r="AD33" s="24"/>
+      <c r="AE33" s="24"/>
+      <c r="AF33" s="24"/>
+    </row>
+    <row r="34" spans="2:32" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="26"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
+      <c r="Q34" s="25"/>
       <c r="R34" s="11"/>
-      <c r="S34" s="26" t="s">
+      <c r="S34" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="T34" s="26"/>
-      <c r="U34" s="26"/>
+      <c r="T34" s="25"/>
+      <c r="U34" s="25"/>
       <c r="V34" s="11"/>
-      <c r="W34" s="26" t="s">
+      <c r="W34" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="X34" s="26"/>
-      <c r="Y34" s="26"/>
-      <c r="Z34" s="26"/>
-      <c r="AA34" s="26"/>
-      <c r="AB34" s="26"/>
-      <c r="AC34" s="26"/>
-      <c r="AD34" s="26"/>
-      <c r="AE34" s="26"/>
-      <c r="AF34" s="26"/>
-    </row>
-    <row r="35" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="X34" s="25"/>
+      <c r="Y34" s="25"/>
+      <c r="Z34" s="25"/>
+      <c r="AA34" s="25"/>
+      <c r="AB34" s="25"/>
+      <c r="AC34" s="25"/>
+      <c r="AD34" s="25"/>
+      <c r="AE34" s="25"/>
+      <c r="AF34" s="25"/>
+    </row>
+    <row r="35" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
@@ -1786,117 +1792,117 @@
       <c r="T35" s="11"/>
       <c r="U35" s="11"/>
       <c r="V35" s="11"/>
-      <c r="W35" s="26"/>
-      <c r="X35" s="26"/>
-      <c r="Y35" s="26"/>
-      <c r="Z35" s="26"/>
-      <c r="AA35" s="26"/>
-      <c r="AB35" s="26"/>
-      <c r="AC35" s="26"/>
-      <c r="AD35" s="26"/>
-      <c r="AE35" s="26"/>
-      <c r="AF35" s="26"/>
-    </row>
-    <row r="36" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
-      <c r="L36" s="29"/>
-      <c r="M36" s="29"/>
-      <c r="N36" s="29"/>
-      <c r="O36" s="29"/>
-      <c r="P36" s="29"/>
-      <c r="Q36" s="29"/>
+      <c r="W35" s="25"/>
+      <c r="X35" s="25"/>
+      <c r="Y35" s="25"/>
+      <c r="Z35" s="25"/>
+      <c r="AA35" s="25"/>
+      <c r="AB35" s="25"/>
+      <c r="AC35" s="25"/>
+      <c r="AD35" s="25"/>
+      <c r="AE35" s="25"/>
+      <c r="AF35" s="25"/>
+    </row>
+    <row r="36" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
       <c r="R36" s="12"/>
-      <c r="S36" s="29"/>
-      <c r="T36" s="29"/>
-      <c r="U36" s="29"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
       <c r="V36" s="12"/>
-      <c r="W36" s="29"/>
-      <c r="X36" s="29"/>
-      <c r="Y36" s="29"/>
-      <c r="Z36" s="29"/>
-      <c r="AA36" s="29"/>
-      <c r="AB36" s="29"/>
-      <c r="AC36" s="29"/>
-      <c r="AD36" s="29"/>
-      <c r="AE36" s="29"/>
-      <c r="AF36" s="29"/>
-    </row>
-    <row r="37" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="17"/>
+      <c r="Y36" s="17"/>
+      <c r="Z36" s="17"/>
+      <c r="AA36" s="17"/>
+      <c r="AB36" s="17"/>
+      <c r="AC36" s="17"/>
+      <c r="AD36" s="17"/>
+      <c r="AE36" s="17"/>
+      <c r="AF36" s="17"/>
+    </row>
+    <row r="37" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
       <c r="R37" s="12"/>
-      <c r="S37" s="29"/>
-      <c r="T37" s="29"/>
-      <c r="U37" s="29"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="17"/>
+      <c r="U37" s="17"/>
       <c r="V37" s="12"/>
-      <c r="W37" s="30"/>
-      <c r="X37" s="30"/>
-      <c r="Y37" s="30"/>
-      <c r="Z37" s="30"/>
-      <c r="AA37" s="30"/>
-      <c r="AB37" s="30"/>
-      <c r="AC37" s="30"/>
-      <c r="AD37" s="30"/>
-      <c r="AE37" s="30"/>
-      <c r="AF37" s="30"/>
-    </row>
-    <row r="38" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="19"/>
+      <c r="Y37" s="19"/>
+      <c r="Z37" s="19"/>
+      <c r="AA37" s="19"/>
+      <c r="AB37" s="19"/>
+      <c r="AC37" s="19"/>
+      <c r="AD37" s="19"/>
+      <c r="AE37" s="19"/>
+      <c r="AF37" s="19"/>
+    </row>
+    <row r="38" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
       <c r="R38" s="4"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
+      <c r="S38" s="17"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="17"/>
       <c r="V38" s="12"/>
-      <c r="W38" s="30"/>
-      <c r="X38" s="30"/>
-      <c r="Y38" s="30"/>
-      <c r="Z38" s="30"/>
-      <c r="AA38" s="30"/>
-      <c r="AB38" s="30"/>
-      <c r="AC38" s="30"/>
-      <c r="AD38" s="30"/>
-      <c r="AE38" s="30"/>
-      <c r="AF38" s="30"/>
-    </row>
-    <row r="39" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
+      <c r="Y38" s="19"/>
+      <c r="Z38" s="19"/>
+      <c r="AA38" s="19"/>
+      <c r="AB38" s="19"/>
+      <c r="AC38" s="19"/>
+      <c r="AD38" s="19"/>
+      <c r="AE38" s="19"/>
+      <c r="AF38" s="19"/>
+    </row>
+    <row r="39" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -1929,33 +1935,33 @@
       <c r="AE39" s="4"/>
       <c r="AF39" s="4"/>
     </row>
-    <row r="40" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B40" s="15" t="s">
+    <row r="40" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B40" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="15"/>
-      <c r="S40" s="15"/>
-      <c r="T40" s="32"/>
-      <c r="U40" s="32"/>
-      <c r="V40" s="32"/>
-      <c r="W40" s="32"/>
-      <c r="X40" s="32"/>
-      <c r="Y40" s="32"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="22"/>
+      <c r="U40" s="22"/>
+      <c r="V40" s="22"/>
+      <c r="W40" s="22"/>
+      <c r="X40" s="22"/>
+      <c r="Y40" s="22"/>
       <c r="Z40" s="14"/>
       <c r="AA40" s="14"/>
       <c r="AB40" s="14"/>
@@ -1964,7 +1970,7 @@
       <c r="AE40" s="14"/>
       <c r="AF40" s="14"/>
     </row>
-    <row r="41" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1997,75 +2003,75 @@
       <c r="AE41" s="2"/>
       <c r="AF41" s="2"/>
     </row>
-    <row r="42" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B42" s="31" t="s">
+    <row r="42" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B42" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="31"/>
-      <c r="M42" s="31"/>
-      <c r="N42" s="31"/>
-      <c r="O42" s="31"/>
-      <c r="P42" s="31"/>
-      <c r="Q42" s="31"/>
-      <c r="R42" s="31"/>
-      <c r="S42" s="31"/>
-      <c r="T42" s="31"/>
-      <c r="U42" s="31"/>
-      <c r="V42" s="31"/>
-      <c r="W42" s="31"/>
-      <c r="X42" s="31"/>
-      <c r="Y42" s="31"/>
-      <c r="Z42" s="31"/>
-      <c r="AA42" s="31"/>
-      <c r="AB42" s="31"/>
-      <c r="AC42" s="31"/>
-      <c r="AD42" s="31"/>
-      <c r="AE42" s="31"/>
-      <c r="AF42" s="31"/>
-    </row>
-    <row r="43" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="31"/>
-      <c r="N43" s="31"/>
-      <c r="O43" s="31"/>
-      <c r="P43" s="31"/>
-      <c r="Q43" s="31"/>
-      <c r="R43" s="31"/>
-      <c r="S43" s="31"/>
-      <c r="T43" s="31"/>
-      <c r="U43" s="31"/>
-      <c r="V43" s="31"/>
-      <c r="W43" s="31"/>
-      <c r="X43" s="31"/>
-      <c r="Y43" s="31"/>
-      <c r="Z43" s="31"/>
-      <c r="AA43" s="31"/>
-      <c r="AB43" s="31"/>
-      <c r="AC43" s="31"/>
-      <c r="AD43" s="31"/>
-      <c r="AE43" s="31"/>
-      <c r="AF43" s="31"/>
-    </row>
-    <row r="44" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="20"/>
+      <c r="U42" s="20"/>
+      <c r="V42" s="20"/>
+      <c r="W42" s="20"/>
+      <c r="X42" s="20"/>
+      <c r="Y42" s="20"/>
+      <c r="Z42" s="20"/>
+      <c r="AA42" s="20"/>
+      <c r="AB42" s="20"/>
+      <c r="AC42" s="20"/>
+      <c r="AD42" s="20"/>
+      <c r="AE42" s="20"/>
+      <c r="AF42" s="20"/>
+    </row>
+    <row r="43" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="20"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="20"/>
+      <c r="Q43" s="20"/>
+      <c r="R43" s="20"/>
+      <c r="S43" s="20"/>
+      <c r="T43" s="20"/>
+      <c r="U43" s="20"/>
+      <c r="V43" s="20"/>
+      <c r="W43" s="20"/>
+      <c r="X43" s="20"/>
+      <c r="Y43" s="20"/>
+      <c r="Z43" s="20"/>
+      <c r="AA43" s="20"/>
+      <c r="AB43" s="20"/>
+      <c r="AC43" s="20"/>
+      <c r="AD43" s="20"/>
+      <c r="AE43" s="20"/>
+      <c r="AF43" s="20"/>
+    </row>
+    <row r="44" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
@@ -2098,42 +2104,42 @@
       <c r="AE44" s="13"/>
       <c r="AF44" s="13"/>
     </row>
-    <row r="46" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B46" s="27" t="s">
+    <row r="46" spans="2:32" ht="15" x14ac:dyDescent="0.25">
+      <c r="B46" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="28"/>
-      <c r="N46" s="28"/>
-      <c r="O46" s="28"/>
-      <c r="P46" s="28"/>
-      <c r="Q46" s="28"/>
-      <c r="R46" s="28"/>
-      <c r="S46" s="28"/>
-      <c r="T46" s="28"/>
-      <c r="U46" s="28"/>
-      <c r="V46" s="28"/>
-      <c r="W46" s="28"/>
-      <c r="X46" s="28"/>
-      <c r="Y46" s="28"/>
-      <c r="Z46" s="28"/>
-      <c r="AA46" s="28"/>
-      <c r="AB46" s="28"/>
-      <c r="AC46" s="28"/>
-      <c r="AD46" s="28"/>
-      <c r="AE46" s="28"/>
-      <c r="AF46" s="28"/>
-    </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+      <c r="T46" s="16"/>
+      <c r="U46" s="16"/>
+      <c r="V46" s="16"/>
+      <c r="W46" s="16"/>
+      <c r="X46" s="16"/>
+      <c r="Y46" s="16"/>
+      <c r="Z46" s="16"/>
+      <c r="AA46" s="16"/>
+      <c r="AB46" s="16"/>
+      <c r="AC46" s="16"/>
+      <c r="AD46" s="16"/>
+      <c r="AE46" s="16"/>
+      <c r="AF46" s="16"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -2149,21 +2155,45 @@
       <c r="N50" s="10"/>
       <c r="O50" s="10"/>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:15" ht="15" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B53" s="5"/>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B54" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="AH19:AN19"/>
+    <mergeCell ref="AB2:AF2"/>
+    <mergeCell ref="B9:AF9"/>
+    <mergeCell ref="B10:AG11"/>
+    <mergeCell ref="B12:AF12"/>
+    <mergeCell ref="F14:L14"/>
+    <mergeCell ref="Y14:AF14"/>
+    <mergeCell ref="AI14:AO14"/>
+    <mergeCell ref="F15:L15"/>
+    <mergeCell ref="AH15:AN15"/>
+    <mergeCell ref="F16:L16"/>
+    <mergeCell ref="AH18:AN18"/>
+    <mergeCell ref="AH20:AN20"/>
+    <mergeCell ref="AH21:AN21"/>
+    <mergeCell ref="AH23:AN23"/>
+    <mergeCell ref="AH24:AN24"/>
+    <mergeCell ref="I26:AF26"/>
+    <mergeCell ref="AH26:AN26"/>
+    <mergeCell ref="I27:AF27"/>
+    <mergeCell ref="I28:AF28"/>
+    <mergeCell ref="B30:AF33"/>
+    <mergeCell ref="B34:Q34"/>
+    <mergeCell ref="S34:U34"/>
+    <mergeCell ref="W34:AF35"/>
     <mergeCell ref="B46:AF46"/>
     <mergeCell ref="B36:Q36"/>
     <mergeCell ref="S36:U36"/>
@@ -2177,30 +2207,6 @@
     <mergeCell ref="B42:AF43"/>
     <mergeCell ref="B40:S40"/>
     <mergeCell ref="T40:Y40"/>
-    <mergeCell ref="I27:AF27"/>
-    <mergeCell ref="I28:AF28"/>
-    <mergeCell ref="B30:AF33"/>
-    <mergeCell ref="B34:Q34"/>
-    <mergeCell ref="S34:U34"/>
-    <mergeCell ref="W34:AF35"/>
-    <mergeCell ref="AH20:AN20"/>
-    <mergeCell ref="AH21:AN21"/>
-    <mergeCell ref="AH23:AN23"/>
-    <mergeCell ref="AH24:AN24"/>
-    <mergeCell ref="I26:AF26"/>
-    <mergeCell ref="AH26:AN26"/>
-    <mergeCell ref="AH19:AN19"/>
-    <mergeCell ref="AB2:AF2"/>
-    <mergeCell ref="B9:AF9"/>
-    <mergeCell ref="B10:AG11"/>
-    <mergeCell ref="B12:AF12"/>
-    <mergeCell ref="F14:L14"/>
-    <mergeCell ref="Y14:AF14"/>
-    <mergeCell ref="AI14:AO14"/>
-    <mergeCell ref="F15:L15"/>
-    <mergeCell ref="AH15:AN15"/>
-    <mergeCell ref="F16:L16"/>
-    <mergeCell ref="AH18:AN18"/>
   </mergeCells>
   <pageMargins left="0.9055118110236221" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="170" scale="93" orientation="portrait" r:id="rId1"/>
@@ -2209,6 +2215,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D262036FF67A5D43BF6E290DEB360352" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c503d2a7b448377a6cc9e75158e3af5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4e744003-367c-4be8-bc40-2385cb622540" xmlns:ns3="0930cf9b-719b-4120-8db4-f84070340397" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9cea96fa3cc1abdf61d90e2bf9fac8d2" ns2:_="" ns3:_="">
     <xsd:import namespace="4e744003-367c-4be8-bc40-2385cb622540"/>
@@ -2425,22 +2446,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CEBEA7B-59B1-46CE-A437-47DAA38AB618}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="0930cf9b-719b-4120-8db4-f84070340397"/>
+    <ds:schemaRef ds:uri="4e744003-367c-4be8-bc40-2385cb622540"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90864A59-6AB3-4A4B-906C-17AADC78847C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3DC5811-E2D9-4774-B143-A47CE40C3F55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2457,29 +2488,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90864A59-6AB3-4A4B-906C-17AADC78847C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CEBEA7B-59B1-46CE-A437-47DAA38AB618}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="0930cf9b-719b-4120-8db4-f84070340397"/>
-    <ds:schemaRef ds:uri="4e744003-367c-4be8-bc40-2385cb622540"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>